<commit_message>
- Added a new parameter sheet "Sheet, with comma", to the Parameters.xlsx and to "TestScenario2" - Update shapshots
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/ModelParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/ModelParameters.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725A3FF-868A-49D2-A5A6-8E1FEFEB530E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23F2110-7F6E-4E34-A95E-F3FC5A35A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="37920" tabRatio="976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
-    <sheet name="MissingParam" sheetId="7" r:id="rId2"/>
-    <sheet name="Aciclovir" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet, with comma" sheetId="8" r:id="rId2"/>
+    <sheet name="MissingParam" sheetId="7" r:id="rId3"/>
+    <sheet name="Aciclovir" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Container Path</t>
   </si>
@@ -398,19 +399,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -443,6 +444,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16AB98-5CE4-407B-B818-A3F5E3A90958}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB1D1D3-9309-4BAC-A19A-8F08944F068E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -450,9 +497,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -482,7 +529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F998E-5869-417D-A696-38B00449383B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -490,9 +537,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -526,26 +573,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -782,26 +809,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -818,4 +846,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Parentheses in parameter sheet names are ignored (#884)
* - Fixes #883
- Parenthesis in parameter sheet names are ignored

* Update tests/testthat/test-utilities-scenario-configuration.R

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

* - Added a new parameter sheet "Sheet, with comma", to the Parameters.xlsx and to "TestScenario2"
- Update shapshots

---------

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/ModelParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/ModelParameters.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725A3FF-868A-49D2-A5A6-8E1FEFEB530E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23F2110-7F6E-4E34-A95E-F3FC5A35A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="37920" tabRatio="976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
-    <sheet name="MissingParam" sheetId="7" r:id="rId2"/>
-    <sheet name="Aciclovir" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet, with comma" sheetId="8" r:id="rId2"/>
+    <sheet name="MissingParam" sheetId="7" r:id="rId3"/>
+    <sheet name="Aciclovir" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Container Path</t>
   </si>
@@ -398,19 +399,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -443,6 +444,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16AB98-5CE4-407B-B818-A3F5E3A90958}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB1D1D3-9309-4BAC-A19A-8F08944F068E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -450,9 +497,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -482,7 +529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F998E-5869-417D-A696-38B00449383B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -490,9 +537,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -526,26 +573,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -782,26 +809,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -818,4 +846,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>